<commit_message>
Rest of the exercises done
</commit_message>
<xml_diff>
--- a/TTC8440tasks.xlsx
+++ b/TTC8440tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REPOSITORIES\oo-programming-ttc8440\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D8D809-5EA8-45EE-88EA-DC47EAC774D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60CAF6C-BDB9-417A-AB92-E3C767720C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="1035" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TasksDone" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>01</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>AA3739</t>
+  </si>
+  <si>
+    <t>T43 Bonus Task</t>
   </si>
 </sst>
 </file>
@@ -682,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED4124D-B70E-458A-9EC1-9C28D6C5FC71}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,6 +1039,9 @@
       <c r="B35" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
@@ -1045,7 +1051,7 @@
         <v>63</v>
       </c>
       <c r="C36" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1056,7 +1062,7 @@
         <v>64</v>
       </c>
       <c r="C37" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1067,7 +1073,7 @@
         <v>65</v>
       </c>
       <c r="C38" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1078,7 +1084,7 @@
         <v>66</v>
       </c>
       <c r="C39" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1089,7 +1095,7 @@
         <v>67</v>
       </c>
       <c r="C40" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1100,7 +1106,7 @@
         <v>68</v>
       </c>
       <c r="C41" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1111,7 +1117,7 @@
         <v>69</v>
       </c>
       <c r="C42" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1122,7 +1128,7 @@
         <v>70</v>
       </c>
       <c r="C43" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1133,7 +1139,7 @@
         <v>71</v>
       </c>
       <c r="C44" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1143,7 +1149,7 @@
       </c>
       <c r="C45" s="10">
         <f>SUM(C35:C44)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1173,7 +1179,7 @@
         <v>38</v>
       </c>
       <c r="C48" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1184,7 +1190,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1195,7 +1201,7 @@
         <v>40</v>
       </c>
       <c r="C50" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1206,7 +1212,7 @@
         <v>41</v>
       </c>
       <c r="C51" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1217,7 +1223,7 @@
         <v>42</v>
       </c>
       <c r="C52" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1228,7 +1234,7 @@
         <v>43</v>
       </c>
       <c r="C53" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1239,7 +1245,7 @@
         <v>44</v>
       </c>
       <c r="C54" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1250,7 +1256,7 @@
         <v>45</v>
       </c>
       <c r="C55" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1261,7 +1267,7 @@
         <v>46</v>
       </c>
       <c r="C56" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1272,7 +1278,7 @@
         <v>47</v>
       </c>
       <c r="C57" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1286,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>42</v>
       </c>
@@ -1294,26 +1300,37 @@
         <v>49</v>
       </c>
       <c r="C59" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>43</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="10">
-        <f>SUM(C48:C59)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="14" t="s">
+      <c r="C61" s="10">
+        <f>SUM(C48:C60)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="15">
-        <f>$C$19+$C$32+$C$45+$C$60</f>
-        <v>20</v>
+      <c r="C63" s="15">
+        <f>$C$19+$C$32+$C$45+$C$61</f>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>